<commit_message>
ApachePOI 2 - MasterThought Parallel Rapor işlemleri - Soru
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/WriteInTheExcelFile.xlsx
+++ b/src/test/java/ApachePOI/resource/WriteInTheExcelFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>Merhaba Dünya</t>
   </si>
@@ -345,7 +345,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -357,6 +357,33 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>9.0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>